<commit_message>
Delete extra lines below code
</commit_message>
<xml_diff>
--- a/data-raw/wp-survey.xlsx
+++ b/data-raw/wp-survey.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/efv_usf_edu/Documents/Accra and Fulbright/Data/Household survey/for owd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/efv_usf_edu/Documents/Data science course/final bug check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{790869B3-2F9F-8548-9C75-70980E40C8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73E42014-1A7D-464F-85C3-F6FA9F6436DE}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{790869B3-2F9F-8548-9C75-70980E40C8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5FDE47D-C3BD-1E4A-A520-4E12FA100196}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{0DA02CE1-17E3-6D40-9DA7-404878CD2691}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{0DA02CE1-17E3-6D40-9DA7-404878CD2691}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,28 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -834,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454A0CFC-5337-FB4D-AC0E-A3378501A2E6}">
-  <dimension ref="A1:AL56"/>
+  <dimension ref="A1:AL50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6084,48 +6062,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="M52" t="str" cm="1">
-        <f t="array" ref="M52:M56">_xlfn.UNIQUE(M2:M50)</f>
-        <v>member(s)_of_owner_household</v>
-      </c>
-      <c r="AA52" t="str" cm="1">
-        <f t="array" ref="AA52:AA56">_xlfn.UNIQUE(AA2:AA50)</f>
-        <v>customers_use_2-liter_bucket_for_bathing,_per-liter_prices_increase_by_33%,_water_point_likely_to_close</v>
-      </c>
-    </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="M53" t="str">
-        <v>employee(s)</v>
-      </c>
-      <c r="AA53" t="str">
-        <v>customers_use_2-liter_bucket_for_bathing,_per-liter_prices_increase_by_33%</v>
-      </c>
-    </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="M54" t="str">
-        <v>member(s)_of_owner_household,employee(s)</v>
-      </c>
-      <c r="AA54" t="str">
-        <v>water_point_likely_to_close</v>
-      </c>
-    </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="M55" t="str">
-        <v>member(s)_of_owner_household,self-managed_or_managed_by_customer(s)</v>
-      </c>
-      <c r="AA55" t="str">
-        <v>n/a</v>
-      </c>
-    </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="M56" t="str">
-        <v>self-managed_or_managed_by_customer(s)</v>
-      </c>
-      <c r="AA56" t="str">
-        <v>customers_use_2-liter_bucket_for_bathing</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>